<commit_message>
Fix underline for Oneida
</commit_message>
<xml_diff>
--- a/py_convert/ZawgyiTest/ZSpreadsheet.xlsx
+++ b/py_convert/ZawgyiTest/ZSpreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -166,7 +166,7 @@
     <font>
       <sz val="44"/>
       <color rgb="FF0000FF"/>
-      <name val="Zawgyi"/>
+      <name val="ZawgyiOne"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -307,8 +307,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="52.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,17 +317,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="2" width="73.91"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="60.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="60.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="60.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -335,17 +335,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="60.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="60.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="60.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -376,8 +376,8 @@
   </sheetPr>
   <dimension ref="A2:B29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -417,7 +417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="145.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="165.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>

</xml_diff>